<commit_message>
Made and exported labware
</commit_message>
<xml_diff>
--- a/tilted_24wp_well_positions.xlsx
+++ b/tilted_24wp_well_positions.xlsx
@@ -460,7 +460,7 @@
         <v>71.67</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>71.67</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.95</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         <v>71.67</v>
       </c>
       <c r="D4" t="n">
-        <v>-5.49</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +508,7 @@
         <v>71.67</v>
       </c>
       <c r="D5" t="n">
-        <v>-8.039999999999999</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="6">
@@ -524,7 +524,7 @@
         <v>71.67</v>
       </c>
       <c r="D6" t="n">
-        <v>-10.58</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="7">
@@ -540,7 +540,7 @@
         <v>71.67</v>
       </c>
       <c r="D7" t="n">
-        <v>-13.13</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="8">
@@ -556,7 +556,7 @@
         <v>52.37</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.4</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="9">
@@ -572,7 +572,7 @@
         <v>52.37</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.95</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="10">
@@ -588,7 +588,7 @@
         <v>52.37</v>
       </c>
       <c r="D10" t="n">
-        <v>-5.49</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="11">
@@ -604,7 +604,7 @@
         <v>52.37</v>
       </c>
       <c r="D11" t="n">
-        <v>-8.039999999999999</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="12">
@@ -620,7 +620,7 @@
         <v>52.37</v>
       </c>
       <c r="D12" t="n">
-        <v>-10.58</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="13">
@@ -636,7 +636,7 @@
         <v>52.37</v>
       </c>
       <c r="D13" t="n">
-        <v>-13.13</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="14">
@@ -652,7 +652,7 @@
         <v>33.07</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.4</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="15">
@@ -668,7 +668,7 @@
         <v>33.07</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.95</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="16">
@@ -684,7 +684,7 @@
         <v>33.07</v>
       </c>
       <c r="D16" t="n">
-        <v>-5.49</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="17">
@@ -700,7 +700,7 @@
         <v>33.07</v>
       </c>
       <c r="D17" t="n">
-        <v>-8.039999999999999</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="18">
@@ -716,7 +716,7 @@
         <v>33.07</v>
       </c>
       <c r="D18" t="n">
-        <v>-10.58</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="19">
@@ -732,7 +732,7 @@
         <v>33.07</v>
       </c>
       <c r="D19" t="n">
-        <v>-13.13</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="20">
@@ -748,7 +748,7 @@
         <v>13.77</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.4</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="21">
@@ -764,7 +764,7 @@
         <v>13.77</v>
       </c>
       <c r="D21" t="n">
-        <v>-2.95</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="22">
@@ -780,7 +780,7 @@
         <v>13.77</v>
       </c>
       <c r="D22" t="n">
-        <v>-5.49</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="23">
@@ -796,7 +796,7 @@
         <v>13.77</v>
       </c>
       <c r="D23" t="n">
-        <v>-8.039999999999999</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="24">
@@ -812,7 +812,7 @@
         <v>13.77</v>
       </c>
       <c r="D24" t="n">
-        <v>-10.58</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="25">
@@ -828,7 +828,7 @@
         <v>13.77</v>
       </c>
       <c r="D25" t="n">
-        <v>-13.13</v>
+        <v>3.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>